<commit_message>
Minor changes before review #1
</commit_message>
<xml_diff>
--- a/Excel/DarsiniTeachers.xlsx
+++ b/Excel/DarsiniTeachers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14868" windowHeight="1572" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14868" windowHeight="1572" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>Class Name</t>
   </si>
@@ -128,12 +128,6 @@
     <t>HOMEFEED CHECK DATA</t>
   </si>
   <si>
-    <t>21/01/2021</t>
-  </si>
-  <si>
-    <t>Central Integration Planner</t>
-  </si>
-  <si>
     <t>Class name</t>
   </si>
   <si>
@@ -170,7 +164,19 @@
     <t>Due Date: 05/03/2021</t>
   </si>
   <si>
-    <t>28/01/2021</t>
+    <t>10/02/2021</t>
+  </si>
+  <si>
+    <t>FeedTestAnnouncement</t>
+  </si>
+  <si>
+    <t>Internal Applications Consultant</t>
+  </si>
+  <si>
+    <t>Feed Test Assignment</t>
+  </si>
+  <si>
+    <t>Test Assignment Desc</t>
   </si>
 </sst>
 </file>
@@ -578,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,38 +691,38 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -724,42 +730,42 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
-        <v>44</v>
-      </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -772,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,38 +872,38 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -905,42 +911,42 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
-        <v>44</v>
-      </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -953,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>